<commit_message>
uploaded 25-Apr all data and code files
</commit_message>
<xml_diff>
--- a/COVID-19/Allformattednumbers.xlsx
+++ b/COVID-19/Allformattednumbers.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="15">
   <si>
     <t>Srikakulam</t>
   </si>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H453"/>
+  <dimension ref="A1:H501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J438" sqref="J438"/>
+    <sheetView tabSelected="1" topLeftCell="A466" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A504" sqref="A504"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -7571,7 +7571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="449" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A449" t="s">
         <v>0</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="450" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A450" t="s">
         <v>2</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A451" t="s">
         <v>1</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="452" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A452" t="s">
         <v>4</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A453" t="s">
         <v>13</v>
       </c>
@@ -7654,6 +7654,723 @@
       </c>
       <c r="E453">
         <v>24</v>
+      </c>
+    </row>
+    <row r="456" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A456" t="s">
+        <v>11</v>
+      </c>
+      <c r="B456">
+        <v>42</v>
+      </c>
+      <c r="C456">
+        <v>32</v>
+      </c>
+      <c r="D456">
+        <v>7</v>
+      </c>
+      <c r="E456">
+        <v>3</v>
+      </c>
+      <c r="H456">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="457" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A457" t="s">
+        <v>9</v>
+      </c>
+      <c r="B457">
+        <v>73</v>
+      </c>
+      <c r="C457">
+        <v>62</v>
+      </c>
+      <c r="D457">
+        <v>11</v>
+      </c>
+      <c r="E457">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="458" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A458" t="s">
+        <v>3</v>
+      </c>
+      <c r="B458">
+        <v>32</v>
+      </c>
+      <c r="C458">
+        <v>24</v>
+      </c>
+      <c r="D458">
+        <v>8</v>
+      </c>
+      <c r="E458">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="459" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A459" t="s">
+        <v>6</v>
+      </c>
+      <c r="B459">
+        <v>195</v>
+      </c>
+      <c r="C459">
+        <v>164</v>
+      </c>
+      <c r="D459">
+        <v>23</v>
+      </c>
+      <c r="E459">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="460" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A460" t="s">
+        <v>10</v>
+      </c>
+      <c r="B460">
+        <v>51</v>
+      </c>
+      <c r="C460">
+        <v>23</v>
+      </c>
+      <c r="D460">
+        <v>28</v>
+      </c>
+      <c r="E460">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="461" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A461" t="s">
+        <v>5</v>
+      </c>
+      <c r="B461">
+        <v>88</v>
+      </c>
+      <c r="C461">
+        <v>56</v>
+      </c>
+      <c r="D461">
+        <v>25</v>
+      </c>
+      <c r="E461">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="462" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A462" t="s">
+        <v>12</v>
+      </c>
+      <c r="B462">
+        <v>234</v>
+      </c>
+      <c r="C462">
+        <v>223</v>
+      </c>
+      <c r="D462">
+        <v>4</v>
+      </c>
+      <c r="E462">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="463" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A463" t="s">
+        <v>8</v>
+      </c>
+      <c r="B463">
+        <v>67</v>
+      </c>
+      <c r="C463">
+        <v>60</v>
+      </c>
+      <c r="D463">
+        <v>6</v>
+      </c>
+      <c r="E463">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="464" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A464" t="s">
+        <v>7</v>
+      </c>
+      <c r="B464">
+        <v>50</v>
+      </c>
+      <c r="C464">
+        <v>48</v>
+      </c>
+      <c r="D464">
+        <v>1</v>
+      </c>
+      <c r="E464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A465" t="s">
+        <v>0</v>
+      </c>
+      <c r="B465">
+        <v>0</v>
+      </c>
+      <c r="C465">
+        <v>0</v>
+      </c>
+      <c r="D465">
+        <v>0</v>
+      </c>
+      <c r="E465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A466" t="s">
+        <v>2</v>
+      </c>
+      <c r="B466">
+        <v>22</v>
+      </c>
+      <c r="C466">
+        <v>3</v>
+      </c>
+      <c r="D466">
+        <v>19</v>
+      </c>
+      <c r="E466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A467" t="s">
+        <v>1</v>
+      </c>
+      <c r="B467">
+        <v>0</v>
+      </c>
+      <c r="C467">
+        <v>0</v>
+      </c>
+      <c r="D467">
+        <v>0</v>
+      </c>
+      <c r="E467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A468" t="s">
+        <v>4</v>
+      </c>
+      <c r="B468">
+        <v>39</v>
+      </c>
+      <c r="C468">
+        <v>30</v>
+      </c>
+      <c r="D468">
+        <v>9</v>
+      </c>
+      <c r="E468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A469" t="s">
+        <v>13</v>
+      </c>
+      <c r="B469">
+        <v>893</v>
+      </c>
+      <c r="C469">
+        <v>725</v>
+      </c>
+      <c r="D469">
+        <v>141</v>
+      </c>
+      <c r="E469">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A472" t="s">
+        <v>11</v>
+      </c>
+      <c r="B472">
+        <v>46</v>
+      </c>
+      <c r="C472">
+        <v>31</v>
+      </c>
+      <c r="D472">
+        <v>11</v>
+      </c>
+      <c r="E472">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A473" t="s">
+        <v>9</v>
+      </c>
+      <c r="B473">
+        <v>73</v>
+      </c>
+      <c r="C473">
+        <v>62</v>
+      </c>
+      <c r="D473">
+        <v>11</v>
+      </c>
+      <c r="E473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A474" t="s">
+        <v>3</v>
+      </c>
+      <c r="B474">
+        <v>34</v>
+      </c>
+      <c r="C474">
+        <v>26</v>
+      </c>
+      <c r="D474">
+        <v>8</v>
+      </c>
+      <c r="E474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A475" t="s">
+        <v>6</v>
+      </c>
+      <c r="B475">
+        <v>206</v>
+      </c>
+      <c r="C475">
+        <v>175</v>
+      </c>
+      <c r="D475">
+        <v>23</v>
+      </c>
+      <c r="E475">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A476" t="s">
+        <v>10</v>
+      </c>
+      <c r="B476">
+        <v>51</v>
+      </c>
+      <c r="C476">
+        <v>23</v>
+      </c>
+      <c r="D476">
+        <v>28</v>
+      </c>
+      <c r="E476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A477" t="s">
+        <v>5</v>
+      </c>
+      <c r="B477">
+        <v>102</v>
+      </c>
+      <c r="C477">
+        <v>70</v>
+      </c>
+      <c r="D477">
+        <v>25</v>
+      </c>
+      <c r="E477">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A478" t="s">
+        <v>12</v>
+      </c>
+      <c r="B478">
+        <v>261</v>
+      </c>
+      <c r="C478">
+        <v>249</v>
+      </c>
+      <c r="D478">
+        <v>4</v>
+      </c>
+      <c r="E478">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A479" t="s">
+        <v>8</v>
+      </c>
+      <c r="B479">
+        <v>68</v>
+      </c>
+      <c r="C479">
+        <v>61</v>
+      </c>
+      <c r="D479">
+        <v>6</v>
+      </c>
+      <c r="E479">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A480" t="s">
+        <v>7</v>
+      </c>
+      <c r="B480">
+        <v>53</v>
+      </c>
+      <c r="C480">
+        <v>51</v>
+      </c>
+      <c r="D480">
+        <v>1</v>
+      </c>
+      <c r="E480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A481" t="s">
+        <v>0</v>
+      </c>
+      <c r="B481">
+        <v>0</v>
+      </c>
+      <c r="C481">
+        <v>0</v>
+      </c>
+      <c r="D481">
+        <v>0</v>
+      </c>
+      <c r="E481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A482" t="s">
+        <v>2</v>
+      </c>
+      <c r="B482">
+        <v>22</v>
+      </c>
+      <c r="C482">
+        <v>3</v>
+      </c>
+      <c r="D482">
+        <v>19</v>
+      </c>
+      <c r="E482">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A483" t="s">
+        <v>1</v>
+      </c>
+      <c r="B483">
+        <v>0</v>
+      </c>
+      <c r="C483">
+        <v>0</v>
+      </c>
+      <c r="D483">
+        <v>0</v>
+      </c>
+      <c r="E483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A484" t="s">
+        <v>4</v>
+      </c>
+      <c r="B484">
+        <v>39</v>
+      </c>
+      <c r="C484">
+        <v>30</v>
+      </c>
+      <c r="D484">
+        <v>9</v>
+      </c>
+      <c r="E484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A485" t="s">
+        <v>13</v>
+      </c>
+      <c r="B485">
+        <v>955</v>
+      </c>
+      <c r="C485">
+        <v>781</v>
+      </c>
+      <c r="D485">
+        <v>145</v>
+      </c>
+      <c r="E485">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A488" t="s">
+        <v>11</v>
+      </c>
+      <c r="B488">
+        <v>51</v>
+      </c>
+      <c r="C488">
+        <v>34</v>
+      </c>
+      <c r="D488">
+        <v>13</v>
+      </c>
+      <c r="E488">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A489" t="s">
+        <v>9</v>
+      </c>
+      <c r="B489">
+        <v>73</v>
+      </c>
+      <c r="C489">
+        <v>62</v>
+      </c>
+      <c r="D489">
+        <v>11</v>
+      </c>
+      <c r="E489">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A490" t="s">
+        <v>3</v>
+      </c>
+      <c r="B490">
+        <v>37</v>
+      </c>
+      <c r="C490">
+        <v>25</v>
+      </c>
+      <c r="D490">
+        <v>12</v>
+      </c>
+      <c r="E490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A491" t="s">
+        <v>6</v>
+      </c>
+      <c r="B491">
+        <v>209</v>
+      </c>
+      <c r="C491">
+        <v>178</v>
+      </c>
+      <c r="D491">
+        <v>23</v>
+      </c>
+      <c r="E491">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A492" t="s">
+        <v>10</v>
+      </c>
+      <c r="B492">
+        <v>55</v>
+      </c>
+      <c r="C492">
+        <v>27</v>
+      </c>
+      <c r="D492">
+        <v>28</v>
+      </c>
+      <c r="E492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A493" t="s">
+        <v>5</v>
+      </c>
+      <c r="B493">
+        <v>127</v>
+      </c>
+      <c r="C493">
+        <v>90</v>
+      </c>
+      <c r="D493">
+        <v>29</v>
+      </c>
+      <c r="E493">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A494" t="s">
+        <v>12</v>
+      </c>
+      <c r="B494">
+        <v>275</v>
+      </c>
+      <c r="C494">
+        <v>259</v>
+      </c>
+      <c r="D494">
+        <v>7</v>
+      </c>
+      <c r="E494">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A495" t="s">
+        <v>8</v>
+      </c>
+      <c r="B495">
+        <v>72</v>
+      </c>
+      <c r="C495">
+        <v>63</v>
+      </c>
+      <c r="D495">
+        <v>8</v>
+      </c>
+      <c r="E495">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A496" t="s">
+        <v>7</v>
+      </c>
+      <c r="B496">
+        <v>53</v>
+      </c>
+      <c r="C496">
+        <v>40</v>
+      </c>
+      <c r="D496">
+        <v>12</v>
+      </c>
+      <c r="E496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A497" t="s">
+        <v>0</v>
+      </c>
+      <c r="B497">
+        <v>3</v>
+      </c>
+      <c r="C497">
+        <v>3</v>
+      </c>
+      <c r="D497">
+        <v>0</v>
+      </c>
+      <c r="E497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A498" t="s">
+        <v>2</v>
+      </c>
+      <c r="B498">
+        <v>22</v>
+      </c>
+      <c r="C498">
+        <v>31</v>
+      </c>
+      <c r="D498">
+        <v>9</v>
+      </c>
+      <c r="E498">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A499" t="s">
+        <v>1</v>
+      </c>
+      <c r="B499">
+        <v>0</v>
+      </c>
+      <c r="C499">
+        <v>0</v>
+      </c>
+      <c r="D499">
+        <v>0</v>
+      </c>
+      <c r="E499">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A500" t="s">
+        <v>4</v>
+      </c>
+      <c r="B500">
+        <v>39</v>
+      </c>
+      <c r="C500">
+        <v>30</v>
+      </c>
+      <c r="D500">
+        <v>9</v>
+      </c>
+      <c r="E500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A501" t="s">
+        <v>13</v>
+      </c>
+      <c r="B501">
+        <v>1016</v>
+      </c>
+      <c r="C501">
+        <v>814</v>
+      </c>
+      <c r="D501">
+        <v>171</v>
+      </c>
+      <c r="E501">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>